<commit_message>
yfinance name extraction + download
</commit_message>
<xml_diff>
--- a/input/SimplifiedFinances_example.xlsx
+++ b/input/SimplifiedFinances_example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nick\Documents\Python Scripts\FinanceAnalysisTools\input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB0B374A-71F7-4AA1-A858-892B064094DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD09FFA0-6374-4581-9F5B-011632C60E04}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="2745" windowWidth="20730" windowHeight="11760" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="17">
   <si>
     <t>Month</t>
   </si>
@@ -71,10 +71,16 @@
     <t>AAPL</t>
   </si>
   <si>
-    <t>Wells Fargo Savings</t>
+    <t>HSA-FTANX</t>
   </si>
   <si>
-    <t>HSA-FTANX</t>
+    <t>Savings-Wells Fargo</t>
+  </si>
+  <si>
+    <t>IRA-FTANX</t>
+  </si>
+  <si>
+    <t>401k-Money Market</t>
   </si>
 </sst>
 </file>
@@ -456,10 +462,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BC999"/>
+  <dimension ref="A1:AZ999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -509,7 +515,7 @@
     <col min="52" max="52" width="18.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -553,14 +559,18 @@
         <v>12</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
@@ -592,10 +602,8 @@
       <c r="AX1" s="2"/>
       <c r="AY1" s="2"/>
       <c r="AZ1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-    </row>
-    <row r="2" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43189</v>
       </c>
@@ -652,7 +660,7 @@
       <c r="AY2" s="5"/>
       <c r="AZ2" s="5"/>
     </row>
-    <row r="3" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43224</v>
       </c>
@@ -708,7 +716,7 @@
       <c r="AY3" s="5"/>
       <c r="AZ3" s="5"/>
     </row>
-    <row r="4" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43258</v>
       </c>
@@ -755,7 +763,7 @@
       <c r="AY4" s="5"/>
       <c r="AZ4" s="5"/>
     </row>
-    <row r="5" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="8"/>
       <c r="B5" s="3"/>
       <c r="G5" s="5"/>
@@ -796,7 +804,7 @@
       <c r="AX5" s="3"/>
       <c r="AY5" s="3"/>
     </row>
-    <row r="6" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="9"/>
       <c r="B6" s="3"/>
       <c r="G6" s="5"/>
@@ -838,7 +846,7 @@
       <c r="AX6" s="6"/>
       <c r="AY6" s="6"/>
     </row>
-    <row r="7" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="9"/>
       <c r="B7" s="3"/>
       <c r="G7" s="5"/>
@@ -876,7 +884,7 @@
       <c r="AX7" s="6"/>
       <c r="AY7" s="6"/>
     </row>
-    <row r="8" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="8"/>
       <c r="B8" s="3"/>
       <c r="G8" s="5"/>
@@ -910,7 +918,7 @@
       <c r="AX8" s="6"/>
       <c r="AY8" s="6"/>
     </row>
-    <row r="9" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="8"/>
       <c r="B9" s="3"/>
       <c r="G9" s="5"/>
@@ -940,7 +948,7 @@
       <c r="AX9" s="6"/>
       <c r="AY9" s="6"/>
     </row>
-    <row r="10" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="8"/>
       <c r="B10" s="3"/>
       <c r="G10" s="5"/>
@@ -970,7 +978,7 @@
       <c r="AX10" s="6"/>
       <c r="AY10" s="6"/>
     </row>
-    <row r="11" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9"/>
       <c r="B11" s="3"/>
       <c r="G11" s="5"/>
@@ -999,7 +1007,7 @@
       <c r="AX11" s="6"/>
       <c r="AY11" s="6"/>
     </row>
-    <row r="12" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="8"/>
       <c r="B12" s="3"/>
       <c r="G12" s="5"/>
@@ -1029,7 +1037,7 @@
       <c r="AX12" s="6"/>
       <c r="AY12" s="6"/>
     </row>
-    <row r="13" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="9"/>
       <c r="B13" s="3"/>
       <c r="G13" s="5"/>
@@ -1058,7 +1066,7 @@
       <c r="AX13" s="6"/>
       <c r="AY13" s="6"/>
     </row>
-    <row r="14" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="8"/>
       <c r="B14" s="3"/>
       <c r="G14" s="5"/>
@@ -1089,7 +1097,7 @@
       <c r="AX14" s="6"/>
       <c r="AY14" s="6"/>
     </row>
-    <row r="15" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="8"/>
       <c r="B15" s="3"/>
       <c r="G15" s="5"/>
@@ -1118,7 +1126,7 @@
       <c r="AX15" s="6"/>
       <c r="AY15" s="6"/>
     </row>
-    <row r="16" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="9"/>
       <c r="B16" s="3"/>
       <c r="G16" s="5"/>
@@ -2324,10 +2332,10 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:BC1000"/>
+  <dimension ref="A1:AZ1000"/>
   <sheetViews>
     <sheetView topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+      <selection activeCell="H1" sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2376,7 +2384,7 @@
     <col min="51" max="51" width="21.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -2420,14 +2428,18 @@
         <v>12</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>
@@ -2459,11 +2471,8 @@
       <c r="AX1" s="2"/>
       <c r="AY1" s="2"/>
       <c r="AZ1" s="2"/>
-      <c r="BA1" s="2"/>
-      <c r="BB1" s="2"/>
-      <c r="BC1" s="2"/>
-    </row>
-    <row r="2" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    </row>
+    <row r="2" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
         <v>43189</v>
       </c>
@@ -2519,7 +2528,7 @@
       <c r="AX2" s="5"/>
       <c r="AY2" s="5"/>
     </row>
-    <row r="3" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
         <v>43224</v>
       </c>
@@ -2574,7 +2583,7 @@
       <c r="AX3" s="5"/>
       <c r="AY3" s="5"/>
     </row>
-    <row r="4" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
         <v>43258</v>
       </c>
@@ -2614,7 +2623,7 @@
       <c r="AX4" s="5"/>
       <c r="AY4" s="5"/>
     </row>
-    <row r="5" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="4"/>
       <c r="B5" s="3"/>
       <c r="C5" s="5"/>
@@ -2651,7 +2660,7 @@
       <c r="AX5" s="3"/>
       <c r="AY5" s="3"/>
     </row>
-    <row r="6" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="7"/>
       <c r="B6" s="3"/>
       <c r="P6" s="6"/>
@@ -2679,7 +2688,7 @@
       <c r="AX6" s="6"/>
       <c r="AY6" s="6"/>
     </row>
-    <row r="7" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="7"/>
       <c r="B7" s="3"/>
       <c r="V7" s="6"/>
@@ -2702,7 +2711,7 @@
       <c r="AX7" s="6"/>
       <c r="AY7" s="6"/>
     </row>
-    <row r="8" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="10"/>
       <c r="B8" s="3"/>
       <c r="C8" s="5"/>
@@ -2722,7 +2731,7 @@
       <c r="AX8" s="6"/>
       <c r="AY8" s="6"/>
     </row>
-    <row r="9" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="10"/>
       <c r="B9" s="3"/>
       <c r="C9" s="5"/>
@@ -2738,7 +2747,7 @@
       <c r="AX9" s="6"/>
       <c r="AY9" s="6"/>
     </row>
-    <row r="10" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="10"/>
       <c r="B10" s="3"/>
       <c r="C10" s="5"/>
@@ -2752,7 +2761,7 @@
       <c r="AX10" s="6"/>
       <c r="AY10" s="6"/>
     </row>
-    <row r="11" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="10"/>
       <c r="B11" s="3"/>
       <c r="C11" s="5"/>
@@ -2767,7 +2776,7 @@
       <c r="AX11" s="6"/>
       <c r="AY11" s="6"/>
     </row>
-    <row r="12" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="7"/>
       <c r="B12" s="3"/>
       <c r="AA12" s="6"/>
@@ -2780,7 +2789,7 @@
       <c r="AX12" s="6"/>
       <c r="AY12" s="6"/>
     </row>
-    <row r="13" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="10"/>
       <c r="B13" s="3"/>
       <c r="C13" s="5"/>
@@ -2794,7 +2803,7 @@
       <c r="AX13" s="6"/>
       <c r="AY13" s="6"/>
     </row>
-    <row r="14" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="7"/>
       <c r="B14" s="3"/>
       <c r="N14" s="6"/>
@@ -2807,7 +2816,7 @@
       <c r="AX14" s="6"/>
       <c r="AY14" s="6"/>
     </row>
-    <row r="15" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="10"/>
       <c r="B15" s="3"/>
       <c r="C15" s="5"/>
@@ -2856,7 +2865,7 @@
       <c r="AX15" s="5"/>
       <c r="AY15" s="5"/>
     </row>
-    <row r="16" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:52" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="11"/>
       <c r="B16" s="3"/>
       <c r="C16" s="5"/>
@@ -4001,8 +4010,8 @@
   </sheetPr>
   <dimension ref="A1:AZ999"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -4094,14 +4103,18 @@
         <v>12</v>
       </c>
       <c r="Q1" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="R1" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="S1" s="1"/>
-      <c r="T1" s="1"/>
-      <c r="U1" s="1"/>
+      <c r="T1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>16</v>
+      </c>
       <c r="V1" s="1"/>
       <c r="W1" s="1"/>
       <c r="X1" s="1"/>

</xml_diff>